<commit_message>
:tada: Enabled to collect company name and Sheet Name.
</commit_message>
<xml_diff>
--- a/public/excel/SaaS_KPI_v0.xlsx
+++ b/public/excel/SaaS_KPI_v0.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/558c6a51a743d5f1/Documents/340_KPI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/558c6a51a743d5f1/GitHub/xlxtractor/public/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="316" documentId="13_ncr:1_{76F330E1-5893-4317-BC11-CAB3B3BCB631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF858723-9FA9-479A-85B9-1E8F151B143F}"/>
+  <xr:revisionPtr revIDLastSave="362" documentId="13_ncr:1_{76F330E1-5893-4317-BC11-CAB3B3BCB631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D01A9BE-2B55-4F60-8DC9-3AA5B5576C50}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{20C6CC3C-5558-49E0-8115-82AE30300C34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{20C6CC3C-5558-49E0-8115-82AE30300C34}"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;Output" sheetId="66" r:id="rId1"/>
     <sheet name="サンプル" sheetId="63" r:id="rId2"/>
-    <sheet name="セル結合" sheetId="61" r:id="rId3"/>
-    <sheet name="空白" sheetId="62" r:id="rId4"/>
-    <sheet name="&gt;Input" sheetId="65" r:id="rId5"/>
-    <sheet name="データ" sheetId="64" r:id="rId6"/>
+    <sheet name="セル結合（列結合）" sheetId="61" r:id="rId3"/>
+    <sheet name="セル結合（行結合）" sheetId="67" r:id="rId4"/>
+    <sheet name="空白" sheetId="62" r:id="rId5"/>
+    <sheet name="&gt;Input" sheetId="65" r:id="rId6"/>
+    <sheet name="データ" sheetId="64" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="支払月">[1]リスト!$B$2:$B$7</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="25">
   <si>
     <t>広告宣伝費</t>
     <rPh sb="0" eb="5">
@@ -163,6 +164,24 @@
   </si>
   <si>
     <t>データ</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>セル結合（行結合）</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>セル結合（列結合）</t>
+    <rPh sb="5" eb="6">
+      <t>レツ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>空白</t>
+    <rPh sb="0" eb="2">
+      <t>クウハク</t>
+    </rPh>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -328,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -507,6 +526,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -558,7 +614,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -672,6 +728,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -996,6 +1067,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1316,7 +1391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8166A696-88B7-46F4-B4FF-1C55D34C1A69}">
   <dimension ref="B2:N13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="51" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1915,7 +1990,7 @@
   <sheetData>
     <row r="2" spans="2:17" ht="20" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2531,6 +2606,636 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29BED591-97DD-48D5-9F28-E4F83A42AD67}">
+  <dimension ref="B2:Q13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="56" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="17" width="10.58203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:17" ht="20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="17">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
+        <v>367</v>
+      </c>
+      <c r="I3" s="4">
+        <v>732</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1097</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1462</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1828</v>
+      </c>
+      <c r="M3" s="4">
+        <v>2193</v>
+      </c>
+      <c r="N3" s="4">
+        <v>2558</v>
+      </c>
+      <c r="O3" s="4">
+        <v>2923</v>
+      </c>
+      <c r="P3" s="4">
+        <v>3289</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>3654</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="6">
+        <f>G5/G9</f>
+        <v>0.27666666666666667</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" ref="H4:Q4" si="0">H5/H9</f>
+        <v>0.33532000000000001</v>
+      </c>
+      <c r="I4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.27093855999999999</v>
+      </c>
+      <c r="J4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.37056492633333332</v>
+      </c>
+      <c r="K4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.51822079698000001</v>
+      </c>
+      <c r="L4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.41872240395984001</v>
+      </c>
+      <c r="M4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.67548065583243633</v>
+      </c>
+      <c r="N4" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1034417043885349</v>
+      </c>
+      <c r="O4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.79091853779074983</v>
+      </c>
+      <c r="P4" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9668106820440425</v>
+      </c>
+      <c r="Q4" s="7">
+        <f t="shared" si="0"/>
+        <v>3.6306720018015475</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="40"/>
+      <c r="C5" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="8">
+        <f>G6*G7/G8</f>
+        <v>83</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" ref="H5:Q5" si="1">H6*H7/H8</f>
+        <v>83.83</v>
+      </c>
+      <c r="I5" s="8">
+        <f t="shared" si="1"/>
+        <v>101.60195999999999</v>
+      </c>
+      <c r="J5" s="8">
+        <f t="shared" si="1"/>
+        <v>111.1694779</v>
+      </c>
+      <c r="K5" s="8">
+        <f t="shared" si="1"/>
+        <v>129.55519924500001</v>
+      </c>
+      <c r="L5" s="8">
+        <f t="shared" si="1"/>
+        <v>157.02090148494</v>
+      </c>
+      <c r="M5" s="8">
+        <f t="shared" si="1"/>
+        <v>202.6441967497309</v>
+      </c>
+      <c r="N5" s="8">
+        <f t="shared" si="1"/>
+        <v>275.86042609713371</v>
+      </c>
+      <c r="O5" s="8">
+        <f t="shared" si="1"/>
+        <v>395.45926889537492</v>
+      </c>
+      <c r="P5" s="8">
+        <f t="shared" si="1"/>
+        <v>590.04320461321277</v>
+      </c>
+      <c r="Q5" s="9">
+        <f t="shared" si="1"/>
+        <v>907.6680004503869</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="42"/>
+      <c r="F6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D6,データ!$B$3:$B$9,0), MATCH(G$3, データ!$B$3:$N$3, 0))</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D6,データ!$B$3:$B$9,0), MATCH(H$3, データ!$B$3:$N$3, 0))</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D6,データ!$B$3:$B$9,0), MATCH(I$3, データ!$B$3:$N$3, 0))</f>
+        <v>1.2</v>
+      </c>
+      <c r="J6" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D6,データ!$B$3:$B$9,0), MATCH(J$3, データ!$B$3:$N$3, 0))</f>
+        <v>1.3</v>
+      </c>
+      <c r="K6" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D6,データ!$B$3:$B$9,0), MATCH(K$3, データ!$B$3:$N$3, 0))</f>
+        <v>1.5</v>
+      </c>
+      <c r="L6" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D6,データ!$B$3:$B$9,0), MATCH(L$3, データ!$B$3:$N$3, 0))</f>
+        <v>1.8</v>
+      </c>
+      <c r="M6" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D6,データ!$B$3:$B$9,0), MATCH(M$3, データ!$B$3:$N$3, 0))</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N6" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D6,データ!$B$3:$B$9,0), MATCH(N$3, データ!$B$3:$N$3, 0))</f>
+        <v>3.1</v>
+      </c>
+      <c r="O6" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D6,データ!$B$3:$B$9,0), MATCH(O$3, データ!$B$3:$N$3, 0))</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P6" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D6,データ!$B$3:$B$9,0), MATCH(P$3, データ!$B$3:$N$3, 0))</f>
+        <v>6.5</v>
+      </c>
+      <c r="Q6" s="24">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D6,データ!$B$3:$B$9,0), MATCH(Q$3, データ!$B$3:$N$3, 0))</f>
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="42"/>
+      <c r="F7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D7,データ!$B$3:$B$9,0), MATCH(G$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.83</v>
+      </c>
+      <c r="H7" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D7,データ!$B$3:$B$9,0), MATCH(H$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.83829999999999993</v>
+      </c>
+      <c r="I7" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D7,データ!$B$3:$B$9,0), MATCH(I$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.84668299999999996</v>
+      </c>
+      <c r="J7" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D7,データ!$B$3:$B$9,0), MATCH(J$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.85514983</v>
+      </c>
+      <c r="K7" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D7,データ!$B$3:$B$9,0), MATCH(K$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.86370132830000002</v>
+      </c>
+      <c r="L7" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D7,データ!$B$3:$B$9,0), MATCH(L$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.87233834158300005</v>
+      </c>
+      <c r="M7" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D7,データ!$B$3:$B$9,0), MATCH(M$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.88106172499883006</v>
+      </c>
+      <c r="N7" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D7,データ!$B$3:$B$9,0), MATCH(N$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.88987234224881839</v>
+      </c>
+      <c r="O7" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D7,データ!$B$3:$B$9,0), MATCH(O$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.8987710656713066</v>
+      </c>
+      <c r="P7" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D7,データ!$B$3:$B$9,0), MATCH(P$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.90775877632801971</v>
+      </c>
+      <c r="Q7" s="24">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D7,データ!$B$3:$B$9,0), MATCH(Q$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.91683636409129987</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="40"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="42"/>
+      <c r="F8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D8,データ!$B$3:$B$9,0), MATCH(G$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.01</v>
+      </c>
+      <c r="H8" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D8,データ!$B$3:$B$9,0), MATCH(H$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.01</v>
+      </c>
+      <c r="I8" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D8,データ!$B$3:$B$9,0), MATCH(I$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.01</v>
+      </c>
+      <c r="J8" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D8,データ!$B$3:$B$9,0), MATCH(J$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.01</v>
+      </c>
+      <c r="K8" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D8,データ!$B$3:$B$9,0), MATCH(K$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.01</v>
+      </c>
+      <c r="L8" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D8,データ!$B$3:$B$9,0), MATCH(L$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.01</v>
+      </c>
+      <c r="M8" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D8,データ!$B$3:$B$9,0), MATCH(M$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.01</v>
+      </c>
+      <c r="N8" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D8,データ!$B$3:$B$9,0), MATCH(N$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.01</v>
+      </c>
+      <c r="O8" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D8,データ!$B$3:$B$9,0), MATCH(O$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.01</v>
+      </c>
+      <c r="P8" s="22">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D8,データ!$B$3:$B$9,0), MATCH(P$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.01</v>
+      </c>
+      <c r="Q8" s="24">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($D8,データ!$B$3:$B$9,0), MATCH(Q$3, データ!$B$3:$N$3, 0))</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="40"/>
+      <c r="C9" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="8">
+        <f>G10/G13</f>
+        <v>300</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" ref="H9:Q9" si="2">H10/H13</f>
+        <v>250</v>
+      </c>
+      <c r="I9" s="8">
+        <f t="shared" si="2"/>
+        <v>375</v>
+      </c>
+      <c r="J9" s="8">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="K9" s="8">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="L9" s="8">
+        <f t="shared" si="2"/>
+        <v>375</v>
+      </c>
+      <c r="M9" s="8">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="N9" s="8">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="O9" s="8">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="P9" s="8">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="Q9" s="9">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="42"/>
+      <c r="F10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="8">
+        <f>G11+G12</f>
+        <v>15000</v>
+      </c>
+      <c r="H10" s="8">
+        <f t="shared" ref="H10:Q10" si="3">H11+H12</f>
+        <v>15000</v>
+      </c>
+      <c r="I10" s="8">
+        <f t="shared" si="3"/>
+        <v>15000</v>
+      </c>
+      <c r="J10" s="8">
+        <f t="shared" si="3"/>
+        <v>15000</v>
+      </c>
+      <c r="K10" s="8">
+        <f t="shared" si="3"/>
+        <v>15000</v>
+      </c>
+      <c r="L10" s="8">
+        <f t="shared" si="3"/>
+        <v>15000</v>
+      </c>
+      <c r="M10" s="8">
+        <f t="shared" si="3"/>
+        <v>15000</v>
+      </c>
+      <c r="N10" s="8">
+        <f t="shared" si="3"/>
+        <v>15000</v>
+      </c>
+      <c r="O10" s="8">
+        <f t="shared" si="3"/>
+        <v>15000</v>
+      </c>
+      <c r="P10" s="8">
+        <f t="shared" si="3"/>
+        <v>15000</v>
+      </c>
+      <c r="Q10" s="9">
+        <f t="shared" si="3"/>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E11,データ!$B$3:$B$9,0), MATCH(G$3, データ!$B$3:$N$3, 0))</f>
+        <v>10000</v>
+      </c>
+      <c r="H11" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E11,データ!$B$3:$B$9,0), MATCH(H$3, データ!$B$3:$N$3, 0))</f>
+        <v>10000</v>
+      </c>
+      <c r="I11" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E11,データ!$B$3:$B$9,0), MATCH(I$3, データ!$B$3:$N$3, 0))</f>
+        <v>10000</v>
+      </c>
+      <c r="J11" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E11,データ!$B$3:$B$9,0), MATCH(J$3, データ!$B$3:$N$3, 0))</f>
+        <v>10000</v>
+      </c>
+      <c r="K11" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E11,データ!$B$3:$B$9,0), MATCH(K$3, データ!$B$3:$N$3, 0))</f>
+        <v>10000</v>
+      </c>
+      <c r="L11" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E11,データ!$B$3:$B$9,0), MATCH(L$3, データ!$B$3:$N$3, 0))</f>
+        <v>10000</v>
+      </c>
+      <c r="M11" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E11,データ!$B$3:$B$9,0), MATCH(M$3, データ!$B$3:$N$3, 0))</f>
+        <v>10000</v>
+      </c>
+      <c r="N11" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E11,データ!$B$3:$B$9,0), MATCH(N$3, データ!$B$3:$N$3, 0))</f>
+        <v>10000</v>
+      </c>
+      <c r="O11" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E11,データ!$B$3:$B$9,0), MATCH(O$3, データ!$B$3:$N$3, 0))</f>
+        <v>10000</v>
+      </c>
+      <c r="P11" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E11,データ!$B$3:$B$9,0), MATCH(P$3, データ!$B$3:$N$3, 0))</f>
+        <v>10000</v>
+      </c>
+      <c r="Q11" s="25">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E11,データ!$B$3:$B$9,0), MATCH(Q$3, データ!$B$3:$N$3, 0))</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E12,データ!$B$3:$B$9,0), MATCH(G$3, データ!$B$3:$N$3, 0))</f>
+        <v>5000</v>
+      </c>
+      <c r="H12" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E12,データ!$B$3:$B$9,0), MATCH(H$3, データ!$B$3:$N$3, 0))</f>
+        <v>5000</v>
+      </c>
+      <c r="I12" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E12,データ!$B$3:$B$9,0), MATCH(I$3, データ!$B$3:$N$3, 0))</f>
+        <v>5000</v>
+      </c>
+      <c r="J12" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E12,データ!$B$3:$B$9,0), MATCH(J$3, データ!$B$3:$N$3, 0))</f>
+        <v>5000</v>
+      </c>
+      <c r="K12" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E12,データ!$B$3:$B$9,0), MATCH(K$3, データ!$B$3:$N$3, 0))</f>
+        <v>5000</v>
+      </c>
+      <c r="L12" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E12,データ!$B$3:$B$9,0), MATCH(L$3, データ!$B$3:$N$3, 0))</f>
+        <v>5000</v>
+      </c>
+      <c r="M12" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E12,データ!$B$3:$B$9,0), MATCH(M$3, データ!$B$3:$N$3, 0))</f>
+        <v>5000</v>
+      </c>
+      <c r="N12" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E12,データ!$B$3:$B$9,0), MATCH(N$3, データ!$B$3:$N$3, 0))</f>
+        <v>5000</v>
+      </c>
+      <c r="O12" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E12,データ!$B$3:$B$9,0), MATCH(O$3, データ!$B$3:$N$3, 0))</f>
+        <v>5000</v>
+      </c>
+      <c r="P12" s="23">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E12,データ!$B$3:$B$9,0), MATCH(P$3, データ!$B$3:$N$3, 0))</f>
+        <v>5000</v>
+      </c>
+      <c r="Q12" s="25">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E12,データ!$B$3:$B$9,0), MATCH(Q$3, データ!$B$3:$N$3, 0))</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="26">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E13,データ!$B$3:$B$9,0), MATCH(G$3, データ!$B$3:$N$3, 0))</f>
+        <v>50</v>
+      </c>
+      <c r="H13" s="26">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E13,データ!$B$3:$B$9,0), MATCH(H$3, データ!$B$3:$N$3, 0))</f>
+        <v>60</v>
+      </c>
+      <c r="I13" s="26">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E13,データ!$B$3:$B$9,0), MATCH(I$3, データ!$B$3:$N$3, 0))</f>
+        <v>40</v>
+      </c>
+      <c r="J13" s="26">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E13,データ!$B$3:$B$9,0), MATCH(J$3, データ!$B$3:$N$3, 0))</f>
+        <v>50</v>
+      </c>
+      <c r="K13" s="26">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E13,データ!$B$3:$B$9,0), MATCH(K$3, データ!$B$3:$N$3, 0))</f>
+        <v>60</v>
+      </c>
+      <c r="L13" s="26">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E13,データ!$B$3:$B$9,0), MATCH(L$3, データ!$B$3:$N$3, 0))</f>
+        <v>40</v>
+      </c>
+      <c r="M13" s="26">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E13,データ!$B$3:$B$9,0), MATCH(M$3, データ!$B$3:$N$3, 0))</f>
+        <v>50</v>
+      </c>
+      <c r="N13" s="26">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E13,データ!$B$3:$B$9,0), MATCH(N$3, データ!$B$3:$N$3, 0))</f>
+        <v>60</v>
+      </c>
+      <c r="O13" s="26">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E13,データ!$B$3:$B$9,0), MATCH(O$3, データ!$B$3:$N$3, 0))</f>
+        <v>30</v>
+      </c>
+      <c r="P13" s="26">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E13,データ!$B$3:$B$9,0), MATCH(P$3, データ!$B$3:$N$3, 0))</f>
+        <v>50</v>
+      </c>
+      <c r="Q13" s="27">
+        <f>INDEX(データ!$B$3:$N$9, MATCH($E13,データ!$B$3:$B$9,0), MATCH(Q$3, データ!$B$3:$N$3, 0))</f>
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="D10:D13"/>
+  </mergeCells>
+  <phoneticPr fontId="5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B91A28-1494-49DA-A8E1-919E9C55EB0B}">
   <dimension ref="B2:Q13"/>
   <sheetViews>
@@ -2546,7 +3251,7 @@
   <sheetData>
     <row r="2" spans="2:17" ht="20" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3152,7 +3857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8B4957-CC23-480E-A10C-BE106511CBE2}">
   <sheetPr>
     <tabColor theme="0" tint="-0.499984740745262"/>
@@ -3195,7 +3900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B2F984-6F39-4399-857B-EDB16AF99A11}">
   <dimension ref="B2:N9"/>
   <sheetViews>

</xml_diff>